<commit_message>
Task Scheduling Document Changed
Nothing important
</commit_message>
<xml_diff>
--- a/Document/Teamwork Cooperation/Task Scheduling.xlsx
+++ b/Document/Teamwork Cooperation/Task Scheduling.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hxsd/Desktop/workspace(Unity)/Fantasy-War/Document/Teamwork Cooperation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hxsd/Desktop/FantasyWarGithubVersion/Fantasy-War/Document/Teamwork Cooperation/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -31,13 +31,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="46">
   <si>
     <t>任务列表</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>完成百分比</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>任务简述/Task Summary</t>
@@ -47,7 +44,7 @@
     <rPh sb="2" eb="3">
       <t>jian'shu</t>
     </rPh>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>任务需求/Task Requirement Description</t>
@@ -57,7 +54,7 @@
     <rPh sb="2" eb="3">
       <t>xu'qiu</t>
     </rPh>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>任务负责人/Task Principal</t>
@@ -70,23 +67,23 @@
     <rPh sb="4" eb="5">
       <t>ren</t>
     </rPh>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>开始日期/Start Date</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>到期日/End Date</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>备注/Remarks</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>任务ID/Task ID</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>游戏框架开发/Frame construction development</t>
@@ -99,7 +96,7 @@
     <rPh sb="4" eb="5">
       <t>kai'fa</t>
     </rPh>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>游戏数据模型自动生成器开发/GamePlay data model automatic generation</t>
@@ -121,7 +118,7 @@
     <rPh sb="11" eb="12">
       <t>kai'fa</t>
     </rPh>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>资源生成管理器/Asset prefab generation manager</t>
@@ -137,7 +134,7 @@
     <rPh sb="6" eb="7">
       <t>qi</t>
     </rPh>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">1.根据指定资源路径生成资源原型，并确保同一个资源不会重复生成多次；
@@ -273,7 +270,7 @@
     <rPh sb="94" eb="95">
       <t>fang'fa</t>
     </rPh>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">1.封装Unity自带的Input函数集，尽量做到完整封装，如果不能确保完整，尽量做到封装规范合理，以便后期迭代新增封装；
@@ -415,7 +412,7 @@
     <rPh sb="113" eb="114">
       <t>feng'zhuang</t>
     </rPh>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">生成器应具备以下功能：
@@ -577,7 +574,7 @@
     <rPh sb="153" eb="154">
       <t>ke'yi</t>
     </rPh>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>输入控制管理器/InputManger</t>
@@ -593,7 +590,7 @@
     <rPh sb="6" eb="7">
       <t>qi</t>
     </rPh>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>对象池管理器/GameObjectManager</t>
@@ -603,7 +600,7 @@
     <rPh sb="3" eb="4">
       <t>guan'li'q</t>
     </rPh>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">1.完成基本的进池、出池逻辑；
@@ -909,14 +906,14 @@
     <rPh sb="201" eb="202">
       <t>xu'y</t>
     </rPh>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>RTS摄像机/RTS Camera</t>
     <rPh sb="3" eb="4">
       <t>she'xiang'ij</t>
     </rPh>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">1.光标在屏幕附近，对应移动摄像机；
@@ -1010,7 +1007,7 @@
     <rPh sb="66" eb="67">
       <t>guan'ce</t>
     </rPh>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>RTS框选功能/RTS Selection</t>
@@ -1020,7 +1017,7 @@
     <rPh sb="5" eb="6">
       <t>gong'n</t>
     </rPh>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>RTS小地图/RTS min map</t>
@@ -1030,7 +1027,7 @@
     <rPh sb="4" eb="5">
       <t>di'tu</t>
     </rPh>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">1.实现方式的运行效率，帧率负荷都可以忽视，先完成功能需求，甚至开第二个摄像机照射也可以；
@@ -1145,7 +1142,7 @@
     <rPh sb="81" eb="82">
       <t>guan'ce</t>
     </rPh>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">1.自动适配鼠标左键单选、左键拖选多选；
@@ -1316,7 +1313,7 @@
     <rPh sb="119" eb="120">
       <t>shi'xian</t>
     </rPh>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>RTS建造建筑物/RTS Building</t>
@@ -1326,7 +1323,7 @@
     <rPh sb="5" eb="6">
       <t>jian'zhu'wu</t>
     </rPh>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>1.设计好暴露给UI以及建筑GameplayLogic的函数接口，尽量保证后期跟其他模块的融合能够顺畅；
@@ -1557,7 +1554,7 @@
     <rPh sb="178" eb="179">
       <t>bian'hua</t>
     </rPh>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>RTS组队编队/RTS Units Teaming</t>
@@ -1567,14 +1564,14 @@
     <rPh sb="5" eb="6">
       <t>bian'dui</t>
     </rPh>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>高</t>
     <rPh sb="0" eb="1">
       <t>gao</t>
     </rPh>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>任务权重/Task Priority</t>
@@ -1584,14 +1581,14 @@
     <rPh sb="2" eb="3">
       <t>quan'zhong</t>
     </rPh>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>低</t>
     <rPh sb="0" eb="1">
       <t>di</t>
     </rPh>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>群体寻路/Multiple Units path finding</t>
@@ -1601,7 +1598,7 @@
     <rPh sb="2" eb="3">
       <t>xun'lu</t>
     </rPh>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>1.50~100个单位同时寻路移动不卡顿，即寻路额外消耗的帧数应不超过10帧（因为假如1方100个单位，2V2就400个单位，如果1方寻路就已经掉10帧，那么剩下3个假设全是AI的话，光寻路最乐观的情况下就要掉40帧，压力已经很大了），在帧率允许的情况下，同时寻路单位数量越多越好；
@@ -1818,14 +1815,14 @@
     <rPh sb="156" eb="157">
       <t>wen'ti</t>
     </rPh>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>中</t>
     <rPh sb="0" eb="1">
       <t>zhong</t>
     </rPh>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>1.框选之后按特定的组合键，能够进行编队，比如框选之后按ctrl+1，那么这次框选的游戏单位，将会被记录为1队，那么不管框选结束还是重新框选，当玩家再次按下1键时，会自动为玩家选择编队1的现存单位，并自动让这些单位变为已选状态;
@@ -2096,14 +2093,14 @@
     <rPh sb="177" eb="178">
       <t>ling'huo'x</t>
     </rPh>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>战争迷雾/War Dense Fog</t>
     <rPh sb="0" eb="1">
       <t>zhan'zheng'mi'wu</t>
     </rPh>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">1.框架应将项目基本Gameplay所需的基类、接口、委托等进行初步的代码实现；
@@ -2290,7 +2287,7 @@
     <rPh sb="133" eb="134">
       <t>gao</t>
     </rPh>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">1.每个己方以及友方单位，提供视野，建筑物、战斗兵种、生成单位提供的视野应该有所区别；
@@ -2435,14 +2432,113 @@
     <rPh sb="106" eb="107">
       <t>shai'xuan</t>
     </rPh>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>李亚丁</t>
+    <rPh sb="0" eb="1">
+      <t>li'ya'ding</t>
+    </rPh>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>完成百分比</t>
+    <rPh sb="0" eb="1">
+      <t>wan'cheng</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>bai'fen'bi</t>
+    </rPh>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>李俊佐</t>
+    <rPh sb="0" eb="1">
+      <t>li'jun'zuo</t>
+    </rPh>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>郑康宇</t>
+    <rPh sb="0" eb="1">
+      <t>zheng'kang'yu</t>
+    </rPh>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>李础翰</t>
+    <rPh sb="0" eb="1">
+      <t>li'chu'han</t>
+    </rPh>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>沈晟</t>
+    <rPh sb="0" eb="1">
+      <t>shen'shen</t>
+    </rPh>
+    <rPh sb="1" eb="2">
+      <t>sheng</t>
+    </rPh>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>矿工动作机与动作机调用脚本/RTSWorkerAnimatorController</t>
+    <rPh sb="0" eb="1">
+      <t>kuang'gong</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>dong'zuo</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>ji</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>yu</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>dong'zuo</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>ji</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>diao'yong</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t>jiao'ben</t>
+    </rPh>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>李俊佐/郑康宇</t>
+    <rPh sb="0" eb="1">
+      <t>li'jun'zuo</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>zheng'kang'yu</t>
+    </rPh>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>RTS单位操作技能面板功能模块/RTSGameUnitActionBehaviourManager</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.负责提供有技能的RTS单位技能控制管理；
+2.独立的面板控制UI逻辑；
+3.能与Demo其他的基础功能模块结合，并不产生行为排斥；
+1.Responsible for providing skilled RTS unit skills control management;
+2.Independent panel control UI logic;
+3.Can combine with other basic functional modules of Demo, and do not produce behavioral exclusion;</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="13"/>
       <color theme="4" tint="0.39991454817346722"/>
@@ -2461,14 +2557,6 @@
       <b/>
       <sz val="13"/>
       <color theme="2"/>
-      <name val="Microsoft YaHei UI"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="4" tint="0.39991454817346722"/>
       <name val="Microsoft YaHei UI"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2504,35 +2592,7 @@
     <font>
       <b/>
       <sz val="20"/>
-      <color rgb="FFFF0000"/>
-      <name val="Microsoft YaHei UI"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="20"/>
       <color rgb="FF00B050"/>
-      <name val="Microsoft YaHei UI"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="20"/>
-      <color rgb="FF00B050"/>
-      <name val="Microsoft YaHei UI"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="20"/>
-      <color theme="4" tint="0.39991454817346722"/>
-      <name val="Microsoft YaHei UI"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="20"/>
-      <color rgb="FFFFC000"/>
       <name val="Microsoft YaHei UI"/>
       <charset val="134"/>
     </font>
@@ -2541,8 +2601,7 @@
       <sz val="20"/>
       <color rgb="FFFFC000"/>
       <name val="Microsoft YaHei UI"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <charset val="134"/>
     </font>
     <font>
       <u/>
@@ -2560,6 +2619,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Microsoft YaHei UI"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Microsoft YaHei UI"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="26"/>
+      <color theme="1"/>
+      <name val="Microsoft YaHei UI"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF24292E"/>
+      <name val="Helvetica"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -2575,7 +2661,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -2592,6 +2678,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -2600,17 +2697,17 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyProtection="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2641,7 +2738,7 @@
     <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
@@ -2659,44 +2756,47 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -2708,20 +2808,44 @@
   </cellStyles>
   <dxfs count="11">
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="26"/>
+        <color theme="1"/>
+        <name val="Microsoft YaHei UI"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="yyyy/m/d"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
-        <b/>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="20"/>
-        <color rgb="FFFF0000"/>
+        <sz val="13"/>
+        <color theme="4" tint="0.39991454817346722"/>
+        <name val="Microsoft YaHei UI"/>
+        <scheme val="minor"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2740,24 +2864,6 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="13"/>
-        <color theme="4" tint="0.39991454817346722"/>
-        <name val="Microsoft YaHei UI"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2875,12 +2981,12 @@
     <tableColumn id="1" name="任务ID/Task ID" dataDxfId="6"/>
     <tableColumn id="9" name="任务简述/Task Summary" dataDxfId="5"/>
     <tableColumn id="3" name="任务需求/Task Requirement Description" dataDxfId="4"/>
-    <tableColumn id="2" name="任务负责人/Task Principal" dataDxfId="3"/>
-    <tableColumn id="10" name="任务权重/Task Priority" dataDxfId="2"/>
+    <tableColumn id="2" name="任务负责人/Task Principal" dataDxfId="2"/>
+    <tableColumn id="10" name="任务权重/Task Priority" dataDxfId="3"/>
     <tableColumn id="4" name="开始日期/Start Date"/>
     <tableColumn id="5" name="到期日/End Date"/>
-    <tableColumn id="6" name="完成百分比" dataDxfId="1"/>
-    <tableColumn id="8" name="备注/Remarks" dataDxfId="0"/>
+    <tableColumn id="6" name="完成百分比" dataDxfId="0"/>
+    <tableColumn id="8" name="备注/Remarks" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="Task List" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -3098,21 +3204,20 @@
     <tabColor theme="4"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A14" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="87" zoomScaleNormal="87" zoomScalePageLayoutView="87" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.875" defaultRowHeight="33" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" style="2" customWidth="1"/>
     <col min="2" max="2" width="41.375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="43.25" style="13" customWidth="1"/>
+    <col min="3" max="3" width="49.875" style="13" customWidth="1"/>
     <col min="4" max="5" width="26" style="2" customWidth="1"/>
     <col min="6" max="6" width="17.875" style="3" customWidth="1"/>
-    <col min="7" max="7" width="15.25" style="3" customWidth="1"/>
-    <col min="8" max="8" width="14.375" style="18" customWidth="1"/>
+    <col min="7" max="8" width="15.25" style="3" customWidth="1"/>
     <col min="9" max="9" width="28.875" style="4" customWidth="1"/>
     <col min="10" max="10" width="2.375" style="1" customWidth="1"/>
     <col min="11" max="16384" width="8.875" style="1"/>
@@ -3128,35 +3233,35 @@
       <c r="E1" s="8"/>
       <c r="F1" s="9"/>
       <c r="G1" s="9"/>
-      <c r="H1" s="16"/>
+      <c r="H1" s="9"/>
     </row>
     <row r="2" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="D2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="E2" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="F2" s="10" t="s">
+      <c r="G2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="H2" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="I2" s="10" t="s">
         <v>6</v>
-      </c>
-      <c r="H2" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="375" customHeight="1" x14ac:dyDescent="0.25">
@@ -3164,14 +3269,16 @@
         <v>0</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="19" t="s">
-        <v>27</v>
+        <v>34</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>26</v>
       </c>
       <c r="F3" s="6">
         <v>43008</v>
@@ -3179,8 +3286,8 @@
       <c r="G3" s="6">
         <v>43021</v>
       </c>
-      <c r="H3" s="20">
-        <v>0</v>
+      <c r="H3" s="26">
+        <v>0.6</v>
       </c>
       <c r="I3" s="5"/>
     </row>
@@ -3189,22 +3296,24 @@
         <v>1</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="22" t="s">
-        <v>29</v>
+        <v>13</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>28</v>
       </c>
       <c r="F4" s="6">
         <v>43008</v>
       </c>
       <c r="G4" s="6">
-        <v>43021</v>
-      </c>
-      <c r="H4" s="25">
+        <v>43038</v>
+      </c>
+      <c r="H4" s="26">
         <v>0</v>
       </c>
       <c r="I4" s="5"/>
@@ -3214,14 +3323,16 @@
         <v>2</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="19" t="s">
-        <v>27</v>
+      <c r="D5" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>26</v>
       </c>
       <c r="F5" s="6">
         <v>43008</v>
@@ -3229,8 +3340,8 @@
       <c r="G5" s="6">
         <v>43021</v>
       </c>
-      <c r="H5" s="21">
-        <v>0</v>
+      <c r="H5" s="26">
+        <v>1</v>
       </c>
       <c r="I5" s="2"/>
     </row>
@@ -3239,13 +3350,16 @@
         <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="19" t="s">
-        <v>27</v>
+        <v>12</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>26</v>
       </c>
       <c r="F6" s="6">
         <v>43008</v>
@@ -3253,8 +3367,8 @@
       <c r="G6" s="6">
         <v>43021</v>
       </c>
-      <c r="H6" s="21">
-        <v>0</v>
+      <c r="H6" s="26">
+        <v>1</v>
       </c>
       <c r="I6" s="2"/>
     </row>
@@ -3263,13 +3377,16 @@
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="19" t="s">
-        <v>27</v>
+      <c r="D7" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>26</v>
       </c>
       <c r="F7" s="6">
         <v>43008</v>
@@ -3277,8 +3394,8 @@
       <c r="G7" s="6">
         <v>43021</v>
       </c>
-      <c r="H7" s="21">
-        <v>0</v>
+      <c r="H7" s="26">
+        <v>0.8</v>
       </c>
       <c r="I7" s="2"/>
     </row>
@@ -3287,13 +3404,16 @@
         <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="19" t="s">
-        <v>27</v>
+      <c r="D8" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>26</v>
       </c>
       <c r="F8" s="6">
         <v>43008</v>
@@ -3301,8 +3421,8 @@
       <c r="G8" s="6">
         <v>43021</v>
       </c>
-      <c r="H8" s="21">
-        <v>0</v>
+      <c r="H8" s="26">
+        <v>0.8</v>
       </c>
       <c r="I8" s="2"/>
     </row>
@@ -3311,13 +3431,16 @@
         <v>6</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" s="19" t="s">
-        <v>27</v>
+      <c r="D9" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>26</v>
       </c>
       <c r="F9" s="6">
         <v>43008</v>
@@ -3325,8 +3448,8 @@
       <c r="G9" s="6">
         <v>43021</v>
       </c>
-      <c r="H9" s="21">
-        <v>0</v>
+      <c r="H9" s="26">
+        <v>0.85</v>
       </c>
       <c r="I9" s="2"/>
     </row>
@@ -3335,13 +3458,16 @@
         <v>7</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="E10" s="19" t="s">
-        <v>27</v>
+        <v>22</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>26</v>
       </c>
       <c r="F10" s="6">
         <v>43008</v>
@@ -3349,8 +3475,8 @@
       <c r="G10" s="6">
         <v>43021</v>
       </c>
-      <c r="H10" s="21">
-        <v>0</v>
+      <c r="H10" s="26">
+        <v>1</v>
       </c>
       <c r="I10" s="2"/>
     </row>
@@ -3359,13 +3485,16 @@
         <v>8</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="E11" s="19" t="s">
-        <v>27</v>
+      <c r="D11" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>26</v>
       </c>
       <c r="F11" s="6">
         <v>43008</v>
@@ -3373,8 +3502,8 @@
       <c r="G11" s="6">
         <v>43021</v>
       </c>
-      <c r="H11" s="21">
-        <v>0</v>
+      <c r="H11" s="26">
+        <v>0.85</v>
       </c>
       <c r="I11" s="2"/>
     </row>
@@ -3383,13 +3512,16 @@
         <v>9</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="16" t="s">
         <v>26</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="E12" s="23" t="s">
-        <v>29</v>
       </c>
       <c r="F12" s="6">
         <v>43008</v>
@@ -3397,8 +3529,8 @@
       <c r="G12" s="6">
         <v>43021</v>
       </c>
-      <c r="H12" s="24">
-        <v>0</v>
+      <c r="H12" s="26">
+        <v>1</v>
       </c>
       <c r="I12" s="2"/>
     </row>
@@ -3407,13 +3539,16 @@
         <v>10</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="D13" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="19" t="s">
         <v>31</v>
-      </c>
-      <c r="E13" s="27" t="s">
-        <v>32</v>
       </c>
       <c r="F13" s="6">
         <v>43008</v>
@@ -3421,8 +3556,8 @@
       <c r="G13" s="6">
         <v>43021</v>
       </c>
-      <c r="H13" s="28">
-        <v>0</v>
+      <c r="H13" s="26">
+        <v>0.85</v>
       </c>
       <c r="I13" s="2"/>
     </row>
@@ -3431,200 +3566,103 @@
         <v>11</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C14" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="E14" s="26"/>
-      <c r="H14" s="21"/>
+      <c r="E14" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14" s="3">
+        <v>43008</v>
+      </c>
+      <c r="G14" s="3">
+        <v>43028</v>
+      </c>
+      <c r="H14" s="27">
+        <v>0.2</v>
+      </c>
       <c r="I14" s="2"/>
+    </row>
+    <row r="15" spans="1:9" ht="308" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="20">
+        <v>12</v>
+      </c>
+      <c r="B15" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="F15" s="23">
+        <v>43008</v>
+      </c>
+      <c r="G15" s="23">
+        <v>43021</v>
+      </c>
+      <c r="H15" s="28">
+        <v>0.8</v>
+      </c>
+      <c r="I15" s="21"/>
+    </row>
+    <row r="16" spans="1:9" ht="308" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="20">
+        <v>13</v>
+      </c>
+      <c r="B16" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="E16" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="F16" s="23">
+        <v>43008</v>
+      </c>
+      <c r="G16" s="23">
+        <v>43021</v>
+      </c>
+      <c r="H16" s="28">
+        <v>0.8</v>
+      </c>
+      <c r="I16" s="21"/>
+    </row>
+    <row r="17" spans="3:3" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C17" s="29"/>
+    </row>
+    <row r="18" spans="3:3" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C18" s="29"/>
+    </row>
+    <row r="19" spans="3:3" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C19" s="29"/>
     </row>
   </sheetData>
   <dataConsolidate/>
-  <phoneticPr fontId="5" type="noConversion"/>
-  <conditionalFormatting sqref="H3:H8 H10">
-    <cfRule type="dataBar" priority="12">
-      <dataBar>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-        <color theme="5"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{E45B70CA-B6A0-4E88-BB95-1D31570318B9}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H9">
-    <cfRule type="dataBar" priority="5">
-      <dataBar>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-        <color theme="5"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{649EFD97-88DF-F147-B39C-5DABFE41A515}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H11">
-    <cfRule type="dataBar" priority="3">
-      <dataBar>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-        <color theme="5"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{15EFD350-63AF-3642-8306-665B16BA95CB}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H12">
-    <cfRule type="dataBar" priority="2">
-      <dataBar>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-        <color theme="5"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{4A5A58E9-E7D1-4841-96BA-F57DE53ED46D}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H13">
-    <cfRule type="dataBar" priority="1">
-      <dataBar>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-        <color theme="5"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{B5F2E9DD-93FB-8341-AB04-81CD260C3786}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <dataValidations count="2">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2">
-      <formula1>0</formula1>
-      <formula2>100</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="这不是列出的值。" error="请在列表中选择一个值。" sqref="H3:H14">
-      <formula1>"0%,25%,50%,75%,100%"</formula1>
-    </dataValidation>
-  </dataValidations>
+  <phoneticPr fontId="4" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.4" right="0.4" top="0.4" bottom="0.4" header="0.25" footer="0.25"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter differentFirst="1">
     <oddFooter>&amp;CPage &amp;P of &amp;N</oddFooter>
   </headerFooter>
-  <ignoredErrors>
-    <ignoredError sqref="H2" listDataValidation="1"/>
-  </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
-      <x14:conditionalFormattings>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{E45B70CA-B6A0-4E88-BB95-1D31570318B9}">
-            <x14:dataBar minLength="0" maxLength="100" border="1" gradient="0" negativeBarBorderColorSameAsPositive="0">
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:borderColor theme="5"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:negativeBorderColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>H3:H8 H10</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{649EFD97-88DF-F147-B39C-5DABFE41A515}">
-            <x14:dataBar minLength="0" maxLength="100" border="1" gradient="0" negativeBarBorderColorSameAsPositive="0">
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:borderColor theme="5"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:negativeBorderColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>H9</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{15EFD350-63AF-3642-8306-665B16BA95CB}">
-            <x14:dataBar minLength="0" maxLength="100" border="1" gradient="0" negativeBarBorderColorSameAsPositive="0">
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:borderColor theme="5"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:negativeBorderColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>H11</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{4A5A58E9-E7D1-4841-96BA-F57DE53ED46D}">
-            <x14:dataBar minLength="0" maxLength="100" border="1" gradient="0" negativeBarBorderColorSameAsPositive="0">
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:borderColor theme="5"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:negativeBorderColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>H12</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{B5F2E9DD-93FB-8341-AB04-81CD260C3786}">
-            <x14:dataBar minLength="0" maxLength="100" border="1" gradient="0" negativeBarBorderColorSameAsPositive="0">
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:borderColor theme="5"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:negativeBorderColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>H13</xm:sqref>
-        </x14:conditionalFormatting>
-      </x14:conditionalFormattings>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -3636,7 +3674,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <sheetData/>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>